<commit_message>
makes activation functional yet it does not do it in a OOP maner
</commit_message>
<xml_diff>
--- a/documentatie/strokenplanning.xlsx
+++ b/documentatie/strokenplanning.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\project 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\project 4\documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D12484A-E3D8-4460-BDAB-7F6EE3B71873}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6378F5-E725-49DF-B518-EC2F3DC96004}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BCB0C761-ACCD-4E55-8E89-099295DC01C8}"/>
   </bookViews>

</xml_diff>